<commit_message>
Agregando comandos para poder manipular usuarios
</commit_message>
<xml_diff>
--- a/assets/Plantilla.xlsx
+++ b/assets/Plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabia\Desktop\acl-manager\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62217EA9-3B30-4650-963F-1A8E0C330B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8EC2D9-1E62-4A18-868E-3CA1B8D686C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>rwx</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>group3</t>
+  </si>
+  <si>
+    <t>/home/redes/Desktop/MartinezRincon-0d5ae8-main</t>
+  </si>
+  <si>
+    <t>/home/redes/Downloads</t>
+  </si>
+  <si>
+    <t>/home/redes/Downloads/Carpeta para probar</t>
   </si>
 </sst>
 </file>
@@ -417,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,6 +466,48 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Acomodando la interfaz del proyecto
</commit_message>
<xml_diff>
--- a/assets/Plantilla.xlsx
+++ b/assets/Plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabia\Desktop\acl-manager\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8EC2D9-1E62-4A18-868E-3CA1B8D686C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E8E22D-1EA3-4443-8CD3-6DA99DEBE08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t>rwx</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>/home/redes/Downloads/Carpeta para probar</t>
+  </si>
+  <si>
+    <t>OTROS</t>
   </si>
 </sst>
 </file>
@@ -426,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,35 +441,41 @@
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -474,18 +483,21 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>0</v>
@@ -493,18 +505,24 @@
       <c r="D4" s="5" t="s">
         <v>0</v>
       </c>
+      <c r="E4" s="5" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregando mas interfaces al proyecto
</commit_message>
<xml_diff>
--- a/assets/Plantilla.xlsx
+++ b/assets/Plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabia\Desktop\acl-manager\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FCA996-EF93-4956-8CF7-B4E63F4F9D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59EEE86-971A-46B1-81FA-FC3D41409857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t>rwx</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>/home/redes/Downloads/Carpeta para probar</t>
+  </si>
+  <si>
+    <t>Otros</t>
   </si>
 </sst>
 </file>
@@ -133,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -145,6 +148,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -426,47 +432,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -474,18 +487,21 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>0</v>
@@ -493,18 +509,24 @@
       <c r="D4" s="5" t="s">
         <v>0</v>
       </c>
+      <c r="E4" s="5" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>